<commit_message>
AITATR3-246 Penambahan section assetdoc
</commit_message>
<xml_diff>
--- a/Excel/2.2 DataFile_NAP_CF4W_Company.xlsx
+++ b/Excel/2.2 DataFile_NAP_CF4W_Company.xlsx
@@ -5,11 +5,11 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fendy.tio\git\NAP-CF4W-UF-NEW\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy.andreas\git\NAP-CF4W-UF-Sprint16\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="769" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="769" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" sheetId="5" r:id="rId1"/>
@@ -2790,7 +2790,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4953" uniqueCount="3615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4958" uniqueCount="3619">
   <si>
     <t>Count</t>
   </si>
@@ -13642,6 +13642,18 @@
   </si>
   <si>
     <t>JOK KULIT</t>
+  </si>
+  <si>
+    <t>Asset Document</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>Document No</t>
+  </si>
+  <si>
+    <t>Document Notes</t>
   </si>
 </sst>
 </file>
@@ -14148,7 +14160,7 @@
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -14370,6 +14382,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -16864,12 +16877,12 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A43" sqref="A43"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1:B2"/>
+      <selection pane="topRight" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18049,23 +18062,37 @@
       </c>
       <c r="H62" s="16"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B63"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B64"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
-      <c r="B65" s="18"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="18"/>
+    <row r="63" spans="1:8" s="139" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="124" t="s">
+        <v>3615</v>
+      </c>
+      <c r="B63" s="125"/>
+    </row>
+    <row r="64" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
+        <v>3616</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
+        <v>3617</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
+        <v>3618</v>
+      </c>
+      <c r="B67" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A11:XFD11"/>
+    <mergeCell ref="A63:XFD63"/>
   </mergeCells>
   <conditionalFormatting sqref="B27:XFD27">
     <cfRule type="expression" dxfId="143" priority="22">
@@ -18180,7 +18207,7 @@
     <dataValidation type="list" errorStyle="information" showInputMessage="1" showErrorMessage="1" sqref="B35:G35">
       <formula1>"REGION1, REGION2, REGION3"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B66 B41:G41">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B41:G41 B66">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="custom" errorStyle="information" showInputMessage="1" showErrorMessage="1" sqref="B45:G45">
@@ -18270,7 +18297,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>IF(B66="Yes",Master!$BX$2:$BX$110)</xm:f>
+            <xm:f>IF(B66="Yes",'[2.1 DataFile_NAP_CF4W.xlsx]Master'!#REF!)</xm:f>
           </x14:formula1>
           <xm:sqref>B65</xm:sqref>
         </x14:dataValidation>
@@ -20199,8 +20226,8 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>